<commit_message>
[Edit] Modification Nom Compétence
</commit_message>
<xml_diff>
--- a/BomberMan.xlsx
+++ b/BomberMan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11715" windowHeight="12075" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11715" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="StatChampion" sheetId="1" r:id="rId1"/>
@@ -238,9 +238,6 @@
     <t>Time Paradox : Le temps est ralenti dans une zone précise</t>
   </si>
   <si>
-    <t>Find Him : Une bombe à tête chercheuse est envoyée sur un joueur, la case du joueur clignote pour laisser à celui-ci le temps de s'enfuir.</t>
-  </si>
-  <si>
     <t>Classique</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>Non</t>
+  </si>
+  <si>
+    <t>Spot Ya! : Une bombe à tête chercheuse est envoyée sur un joueur, la case du joueur clignote pour laisser à celui-ci le temps de s'enfuir.</t>
   </si>
 </sst>
 </file>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +900,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>41</v>
       </c>
@@ -929,7 +929,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>42</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>60</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1076,21 +1076,21 @@
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>